<commit_message>
Divide functions from manager.py
- create py file by functions from manager.py
</commit_message>
<xml_diff>
--- a/1학년 1반.xlsx
+++ b/1학년 1반.xlsx
@@ -359,11 +359,7 @@
           <t>민준</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">잘하자 잘했다 </t>
-        </is>
-      </c>
+      <c r="B1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -373,7 +369,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>바보다 보통이다 괜찮다</t>
+          <t>보통이야</t>
         </is>
       </c>
     </row>
@@ -385,7 +381,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>그저 그렇다 실망쓰! 최악이다</t>
+          <t>바보야!</t>
         </is>
       </c>
     </row>
@@ -397,7 +393,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>뛰어나다 괜찮다</t>
+          <t>보통이야</t>
         </is>
       </c>
     </row>
@@ -407,11 +403,7 @@
           <t>지훈</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>최고다 괜찮다</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -419,11 +411,7 @@
           <t>도현</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>그저 그렇다 완벽하다</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -431,11 +419,7 @@
           <t>우진</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>더 잘해라 완벽하다</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -443,11 +427,7 @@
           <t>선우</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>실망이다</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">

</xml_diff>